<commit_message>
debug savukosky et affichage de seulement le graphe de moyenne ( au mois et à l'année)
</commit_message>
<xml_diff>
--- a/Savukoski_kirkonkyla.xlsx
+++ b/Savukoski_kirkonkyla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TP_QualiteDesDonnees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFF837F-A491-4374-9B40-AABA60A21E14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B752B-B82B-4BFC-835B-ABA24BAFD073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="74">
   <si>
     <t>Observation station</t>
   </si>
@@ -216,6 +216,48 @@
   </si>
   <si>
     <t>jour_max</t>
+  </si>
+  <si>
+    <t>janvier_median</t>
+  </si>
+  <si>
+    <t>mars_median</t>
+  </si>
+  <si>
+    <t>avril_median</t>
+  </si>
+  <si>
+    <t>mai_median</t>
+  </si>
+  <si>
+    <t>juin_median</t>
+  </si>
+  <si>
+    <t>juillet_median</t>
+  </si>
+  <si>
+    <t>août_median</t>
+  </si>
+  <si>
+    <t>septembre_median</t>
+  </si>
+  <si>
+    <t>octobre_median</t>
+  </si>
+  <si>
+    <t>jour_median</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>février_median</t>
+  </si>
+  <si>
+    <t>novembre_median</t>
+  </si>
+  <si>
+    <t>décembre_median</t>
   </si>
 </sst>
 </file>
@@ -10239,10 +10281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655AA9EA-45A1-4433-AD1D-A9EF4F799619}">
-  <dimension ref="B1:AG368"/>
+  <dimension ref="B1:AT366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AH367"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AO21" sqref="AO21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10253,7 +10295,7 @@
     <col min="28" max="28" width="13.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>58</v>
       </c>
@@ -10344,8 +10386,47 @@
       <c r="AG1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD2">
         <v>1</v>
       </c>
@@ -10358,8 +10439,11 @@
       <c r="AG2">
         <v>-4</v>
       </c>
-    </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AI2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -10450,8 +10534,59 @@
       <c r="AG3">
         <v>-4.5999999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <f>(C3+Q3)/2</f>
+        <v>-3.35</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3:AT18" si="0">(D3+R3)/2</f>
+        <v>-26.200000000000003</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" si="0"/>
+        <v>-9.9499999999999993</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="0"/>
+        <v>-6.4499999999999993</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" si="0"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" si="0"/>
+        <v>12.65</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" si="0"/>
+        <v>11.95</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" si="0"/>
+        <v>24.049999999999997</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" si="0"/>
+        <v>2.85</v>
+      </c>
+      <c r="AS3">
+        <f t="shared" si="0"/>
+        <v>1.95</v>
+      </c>
+      <c r="AT3">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -10542,8 +10677,59 @@
       <c r="AG4">
         <v>-4.4000000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH4">
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" ref="AI4:AI33" si="1">(C4+Q4)/2</f>
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="0"/>
+        <v>-22.75</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="0"/>
+        <v>-7.3000000000000007</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="0"/>
+        <v>-7.9499999999999993</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="0"/>
+        <v>9.85</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="0"/>
+        <v>16.3</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" si="0"/>
+        <v>21.3</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="0"/>
+        <v>13.25</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" si="0"/>
+        <v>-0.44999999999999996</v>
+      </c>
+      <c r="AS4">
+        <f t="shared" si="0"/>
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AT4">
+        <f t="shared" si="0"/>
+        <v>-2.35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -10634,8 +10820,59 @@
       <c r="AG5">
         <v>-6.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH5">
+        <v>3</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="1"/>
+        <v>-3.95</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="0"/>
+        <v>-17.45</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="0"/>
+        <v>-14.35</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="0"/>
+        <v>-2.6</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="0"/>
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="0"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" si="0"/>
+        <v>-2.8499999999999996</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" si="0"/>
+        <v>-0.65</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" si="0"/>
+        <v>-3.1500000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -10726,8 +10963,59 @@
       <c r="AG6">
         <v>-11.2</v>
       </c>
-    </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="1"/>
+        <v>-5.95</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="0"/>
+        <v>-21.7</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" si="0"/>
+        <v>-18.05</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" si="0"/>
+        <v>-0.54999999999999982</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="0"/>
+        <v>5.55</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="0"/>
+        <v>15.85</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="0"/>
+        <v>13.75</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="0"/>
+        <v>11.75</v>
+      </c>
+      <c r="AR6">
+        <f t="shared" si="0"/>
+        <v>-1.4500000000000002</v>
+      </c>
+      <c r="AS6">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="AT6">
+        <f t="shared" si="0"/>
+        <v>-4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -10818,8 +11106,59 @@
       <c r="AG7">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH7">
+        <v>5</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="1"/>
+        <v>-10.9</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" si="0"/>
+        <v>-27.2</v>
+      </c>
+      <c r="AK7">
+        <f t="shared" si="0"/>
+        <v>-16.850000000000001</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="0"/>
+        <v>-1.2500000000000002</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="0"/>
+        <v>14.600000000000001</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="0"/>
+        <v>10.3</v>
+      </c>
+      <c r="AR7">
+        <f t="shared" si="0"/>
+        <v>-3.3</v>
+      </c>
+      <c r="AS7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="AT7">
+        <f t="shared" si="0"/>
+        <v>-4.5500000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -10910,8 +11249,59 @@
       <c r="AG8">
         <v>-6</v>
       </c>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH8">
+        <v>6</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="1"/>
+        <v>-3.55</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="0"/>
+        <v>-21.6</v>
+      </c>
+      <c r="AK8">
+        <f t="shared" si="0"/>
+        <v>-20.65</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="0"/>
+        <v>17.149999999999999</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="0"/>
+        <v>13.15</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" si="0"/>
+        <v>10.35</v>
+      </c>
+      <c r="AR8">
+        <f t="shared" si="0"/>
+        <v>-1.8499999999999999</v>
+      </c>
+      <c r="AS8">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="AT8">
+        <f t="shared" si="0"/>
+        <v>-4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -11002,8 +11392,59 @@
       <c r="AG9">
         <v>-11.7</v>
       </c>
-    </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="1"/>
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="0"/>
+        <v>-15</v>
+      </c>
+      <c r="AK9">
+        <f t="shared" si="0"/>
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="0"/>
+        <v>-0.95</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="0"/>
+        <v>10.25</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="0"/>
+        <v>8.1</v>
+      </c>
+      <c r="AR9">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="AS9">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="AT9">
+        <f t="shared" si="0"/>
+        <v>-8.85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -11094,8 +11535,59 @@
       <c r="AG10">
         <v>-13</v>
       </c>
-    </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH10">
+        <v>8</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="1"/>
+        <v>-12.8</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="0"/>
+        <v>-17.049999999999997</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="0"/>
+        <v>-15.05</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" si="0"/>
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="0"/>
+        <v>6.15</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" si="0"/>
+        <v>14.6</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" si="0"/>
+        <v>6.6499999999999995</v>
+      </c>
+      <c r="AR10">
+        <f t="shared" si="0"/>
+        <v>-3.95</v>
+      </c>
+      <c r="AS10">
+        <f t="shared" si="0"/>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="AT10">
+        <f t="shared" si="0"/>
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -11186,8 +11678,59 @@
       <c r="AG11">
         <v>-8.9</v>
       </c>
-    </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH11">
+        <v>9</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="1"/>
+        <v>-11.4</v>
+      </c>
+      <c r="AJ11">
+        <f t="shared" si="0"/>
+        <v>-9.9</v>
+      </c>
+      <c r="AK11">
+        <f t="shared" si="0"/>
+        <v>-9.6</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="0"/>
+        <v>-6.5</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="0"/>
+        <v>8.15</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="0"/>
+        <v>7.6</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="0"/>
+        <v>17.3</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="0"/>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="AR11">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AS11">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="AT11">
+        <f t="shared" si="0"/>
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -11278,8 +11821,59 @@
       <c r="AG12">
         <v>-6.2</v>
       </c>
-    </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH12">
+        <v>10</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="1"/>
+        <v>-10.7</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="0"/>
+        <v>-6.35</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="0"/>
+        <v>-6.9499999999999993</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="0"/>
+        <v>-1.5000000000000002</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="0"/>
+        <v>13.65</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="0"/>
+        <v>9.35</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="0"/>
+        <v>17.7</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="0"/>
+        <v>16.850000000000001</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="0"/>
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="AR12">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="AS12">
+        <f t="shared" si="0"/>
+        <v>-0.35</v>
+      </c>
+      <c r="AT12">
+        <f t="shared" si="0"/>
+        <v>-2.35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -11370,8 +11964,59 @@
       <c r="AG13">
         <v>-6.5</v>
       </c>
-    </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH13">
+        <v>11</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="1"/>
+        <v>-5.95</v>
+      </c>
+      <c r="AJ13">
+        <f t="shared" si="0"/>
+        <v>-7.8</v>
+      </c>
+      <c r="AK13">
+        <f t="shared" si="0"/>
+        <v>-3.35</v>
+      </c>
+      <c r="AL13">
+        <f t="shared" si="0"/>
+        <v>-1.8500000000000005</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="0"/>
+        <v>11.75</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="0"/>
+        <v>19.850000000000001</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="0"/>
+        <v>17.45</v>
+      </c>
+      <c r="AQ13">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+      <c r="AR13">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AS13">
+        <f t="shared" si="0"/>
+        <v>-0.6</v>
+      </c>
+      <c r="AT13">
+        <f t="shared" si="0"/>
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -11462,8 +12107,59 @@
       <c r="AG14">
         <v>-10.1</v>
       </c>
-    </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH14">
+        <v>12</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="AJ14">
+        <f t="shared" si="0"/>
+        <v>-12.85</v>
+      </c>
+      <c r="AK14">
+        <f t="shared" si="0"/>
+        <v>-6.65</v>
+      </c>
+      <c r="AL14">
+        <f t="shared" si="0"/>
+        <v>-0.25</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="0"/>
+        <v>14.05</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="0"/>
+        <v>4.8500000000000005</v>
+      </c>
+      <c r="AO14">
+        <f t="shared" si="0"/>
+        <v>19.7</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AQ14">
+        <f t="shared" si="0"/>
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="AR14">
+        <f t="shared" si="0"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AS14">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="AT14">
+        <f t="shared" si="0"/>
+        <v>-11.65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -11554,8 +12250,59 @@
       <c r="AG15">
         <v>-3</v>
       </c>
-    </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH15">
+        <v>13</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="1"/>
+        <v>-10.149999999999999</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="0"/>
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="AK15">
+        <f t="shared" si="0"/>
+        <v>-9.35</v>
+      </c>
+      <c r="AL15">
+        <f t="shared" si="0"/>
+        <v>-0.79999999999999982</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="0"/>
+        <v>14.55</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="0"/>
+        <v>5.9</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="0"/>
+        <v>18.350000000000001</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="0"/>
+        <v>10.899999999999999</v>
+      </c>
+      <c r="AR15">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999996</v>
+      </c>
+      <c r="AT15">
+        <f t="shared" si="0"/>
+        <v>-12.450000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -11646,8 +12393,59 @@
       <c r="AG16">
         <v>-5.3</v>
       </c>
-    </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH16">
+        <v>14</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" si="1"/>
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="AJ16">
+        <f t="shared" si="0"/>
+        <v>-3.3</v>
+      </c>
+      <c r="AK16">
+        <f t="shared" si="0"/>
+        <v>-8.8000000000000007</v>
+      </c>
+      <c r="AL16">
+        <f t="shared" si="0"/>
+        <v>2.0500000000000003</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="0"/>
+        <v>15.35</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="0"/>
+        <v>9.7000000000000011</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="0"/>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="0"/>
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
+      </c>
+      <c r="AR16">
+        <f t="shared" si="0"/>
+        <v>10.25</v>
+      </c>
+      <c r="AS16">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="AT16">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
@@ -11738,8 +12536,59 @@
       <c r="AG17">
         <v>-11.2</v>
       </c>
-    </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH17">
+        <v>15</v>
+      </c>
+      <c r="AI17">
+        <f t="shared" si="1"/>
+        <v>-5.25</v>
+      </c>
+      <c r="AJ17">
+        <f t="shared" si="0"/>
+        <v>-2.35</v>
+      </c>
+      <c r="AK17">
+        <f t="shared" si="0"/>
+        <v>-14.350000000000001</v>
+      </c>
+      <c r="AL17">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="0"/>
+        <v>14.9</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="0"/>
+        <v>18.850000000000001</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="0"/>
+        <v>10.25</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AR17">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="AS17">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="AT17">
+        <f t="shared" si="0"/>
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -11830,8 +12679,59 @@
       <c r="AG18">
         <v>-15.8</v>
       </c>
-    </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH18">
+        <v>16</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="1"/>
+        <v>-10.050000000000001</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="0"/>
+        <v>-5.25</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="0"/>
+        <v>-13.75</v>
+      </c>
+      <c r="AL18">
+        <f t="shared" si="0"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="0"/>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="AR18">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="AS18">
+        <f t="shared" si="0"/>
+        <v>3.85</v>
+      </c>
+      <c r="AT18">
+        <f t="shared" si="0"/>
+        <v>-5.55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
@@ -11922,8 +12822,59 @@
       <c r="AG19">
         <v>-10.5</v>
       </c>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH19">
+        <v>17</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" si="1"/>
+        <v>-15.5</v>
+      </c>
+      <c r="AJ19">
+        <f t="shared" ref="AJ19:AJ33" si="2">(D19+R19)/2</f>
+        <v>-8.25</v>
+      </c>
+      <c r="AK19">
+        <f t="shared" ref="AK19:AK33" si="3">(E19+S19)/2</f>
+        <v>-11.200000000000001</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" ref="AL19:AL33" si="4">(F19+T19)/2</f>
+        <v>6.05</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" ref="AM19:AM33" si="5">(G19+U19)/2</f>
+        <v>10.5</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" ref="AN19:AN33" si="6">(H19+V19)/2</f>
+        <v>14.55</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" ref="AO19:AO33" si="7">(I19+W19)/2</f>
+        <v>21.6</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" ref="AP19:AP33" si="8">(J19+X19)/2</f>
+        <v>16.7</v>
+      </c>
+      <c r="AQ19">
+        <f t="shared" ref="AQ19:AQ33" si="9">(K19+Y19)/2</f>
+        <v>7</v>
+      </c>
+      <c r="AR19">
+        <f t="shared" ref="AR19:AR33" si="10">(L19+Z19)/2</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AS19">
+        <f t="shared" ref="AS19:AS33" si="11">(M19+AA19)/2</f>
+        <v>3.65</v>
+      </c>
+      <c r="AT19">
+        <f t="shared" ref="AT19:AT33" si="12">(N19+AB19)/2</f>
+        <v>-6.55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>18</v>
       </c>
@@ -12014,8 +12965,59 @@
       <c r="AG20">
         <v>-14</v>
       </c>
-    </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH20">
+        <v>18</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="1"/>
+        <v>-11.55</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" si="2"/>
+        <v>-14.100000000000001</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" si="3"/>
+        <v>-3.05</v>
+      </c>
+      <c r="AL20">
+        <f t="shared" si="4"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="5"/>
+        <v>7.45</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="6"/>
+        <v>15.75</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="7"/>
+        <v>24.7</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="8"/>
+        <v>17.45</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" si="9"/>
+        <v>6.2</v>
+      </c>
+      <c r="AR20">
+        <f t="shared" si="10"/>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="AS20">
+        <f t="shared" si="11"/>
+        <v>-1.7</v>
+      </c>
+      <c r="AT20">
+        <f t="shared" si="12"/>
+        <v>-7.15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>19</v>
       </c>
@@ -12100,8 +13102,55 @@
       <c r="AG21">
         <v>-11.5</v>
       </c>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH21">
+        <v>19</v>
+      </c>
+      <c r="AI21">
+        <f t="shared" si="1"/>
+        <v>-13.35</v>
+      </c>
+      <c r="AJ21">
+        <f t="shared" si="2"/>
+        <v>-19</v>
+      </c>
+      <c r="AK21">
+        <f t="shared" si="3"/>
+        <v>-10.600000000000001</v>
+      </c>
+      <c r="AL21">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="5"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="6"/>
+        <v>15.5</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="8"/>
+        <v>14.700000000000001</v>
+      </c>
+      <c r="AQ21">
+        <f t="shared" si="9"/>
+        <v>5.7</v>
+      </c>
+      <c r="AR21">
+        <f t="shared" si="10"/>
+        <v>0.8</v>
+      </c>
+      <c r="AS21">
+        <f t="shared" si="11"/>
+        <v>-5.05</v>
+      </c>
+      <c r="AT21">
+        <f t="shared" si="12"/>
+        <v>-6.9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20</v>
       </c>
@@ -12186,8 +13235,55 @@
       <c r="AG22">
         <v>-13.3</v>
       </c>
-    </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH22">
+        <v>20</v>
+      </c>
+      <c r="AI22">
+        <f t="shared" si="1"/>
+        <v>-13.85</v>
+      </c>
+      <c r="AJ22">
+        <f t="shared" si="2"/>
+        <v>-21.5</v>
+      </c>
+      <c r="AK22">
+        <f t="shared" si="3"/>
+        <v>-15.549999999999999</v>
+      </c>
+      <c r="AL22">
+        <f t="shared" si="4"/>
+        <v>-1.2</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="5"/>
+        <v>9.9</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="6"/>
+        <v>12.85</v>
+      </c>
+      <c r="AP22">
+        <f t="shared" si="8"/>
+        <v>11.1</v>
+      </c>
+      <c r="AQ22">
+        <f t="shared" si="9"/>
+        <v>9.75</v>
+      </c>
+      <c r="AR22">
+        <f t="shared" si="10"/>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="AS22">
+        <f t="shared" si="11"/>
+        <v>-1.2999999999999998</v>
+      </c>
+      <c r="AT22">
+        <f t="shared" si="12"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>21</v>
       </c>
@@ -12278,8 +13374,59 @@
       <c r="AG23">
         <v>-21</v>
       </c>
-    </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH23">
+        <v>21</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" si="1"/>
+        <v>-11.5</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" si="2"/>
+        <v>-17.75</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" si="3"/>
+        <v>-14.95</v>
+      </c>
+      <c r="AL23">
+        <f t="shared" si="4"/>
+        <v>-1.3499999999999999</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="5"/>
+        <v>14.8</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="6"/>
+        <v>11.850000000000001</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="7"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="9"/>
+        <v>10.75</v>
+      </c>
+      <c r="AR23">
+        <f t="shared" si="10"/>
+        <v>3.25</v>
+      </c>
+      <c r="AS23">
+        <f t="shared" si="11"/>
+        <v>-0.49999999999999994</v>
+      </c>
+      <c r="AT23">
+        <f t="shared" si="12"/>
+        <v>-9.5500000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>22</v>
       </c>
@@ -12370,8 +13517,59 @@
       <c r="AG24">
         <v>-22.2</v>
       </c>
-    </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH24">
+        <v>22</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" si="1"/>
+        <v>-19.95</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" si="2"/>
+        <v>-16.799999999999997</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" si="3"/>
+        <v>-7.5</v>
+      </c>
+      <c r="AL24">
+        <f t="shared" si="4"/>
+        <v>-1.0999999999999999</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="5"/>
+        <v>15.5</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="6"/>
+        <v>11.049999999999999</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="7"/>
+        <v>21.3</v>
+      </c>
+      <c r="AP24">
+        <f t="shared" si="8"/>
+        <v>8.25</v>
+      </c>
+      <c r="AQ24">
+        <f t="shared" si="9"/>
+        <v>12.15</v>
+      </c>
+      <c r="AR24">
+        <f t="shared" si="10"/>
+        <v>1.6999999999999997</v>
+      </c>
+      <c r="AS24">
+        <f t="shared" si="11"/>
+        <v>-0.95</v>
+      </c>
+      <c r="AT24">
+        <f t="shared" si="12"/>
+        <v>-18.649999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>23</v>
       </c>
@@ -12462,8 +13660,59 @@
       <c r="AG25">
         <v>-22.5</v>
       </c>
-    </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH25">
+        <v>23</v>
+      </c>
+      <c r="AI25">
+        <f t="shared" si="1"/>
+        <v>-23.15</v>
+      </c>
+      <c r="AJ25">
+        <f t="shared" si="2"/>
+        <v>-22.7</v>
+      </c>
+      <c r="AK25">
+        <f t="shared" si="3"/>
+        <v>-13</v>
+      </c>
+      <c r="AL25">
+        <f t="shared" si="4"/>
+        <v>2.65</v>
+      </c>
+      <c r="AM25">
+        <f t="shared" si="5"/>
+        <v>11.45</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="6"/>
+        <v>11.55</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="7"/>
+        <v>21.85</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="8"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="AQ25">
+        <f t="shared" si="9"/>
+        <v>9.6</v>
+      </c>
+      <c r="AR25">
+        <f t="shared" si="10"/>
+        <v>-3.9499999999999997</v>
+      </c>
+      <c r="AS25">
+        <f t="shared" si="11"/>
+        <v>-4.2</v>
+      </c>
+      <c r="AT25">
+        <f t="shared" si="12"/>
+        <v>-24.8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>24</v>
       </c>
@@ -12554,8 +13803,59 @@
       <c r="AG26">
         <v>-4</v>
       </c>
-    </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH26">
+        <v>24</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="1"/>
+        <v>-23.35</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="2"/>
+        <v>-22.35</v>
+      </c>
+      <c r="AK26">
+        <f t="shared" si="3"/>
+        <v>-7.95</v>
+      </c>
+      <c r="AL26">
+        <f t="shared" si="4"/>
+        <v>4.25</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="6"/>
+        <v>11.55</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="7"/>
+        <v>21.4</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="8"/>
+        <v>9.4</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="9"/>
+        <v>5.7</v>
+      </c>
+      <c r="AR26">
+        <f t="shared" si="10"/>
+        <v>-5</v>
+      </c>
+      <c r="AS26">
+        <f t="shared" si="11"/>
+        <v>-2.1</v>
+      </c>
+      <c r="AT26">
+        <f t="shared" si="12"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>25</v>
       </c>
@@ -12646,8 +13946,59 @@
       <c r="AG27">
         <v>-12.1</v>
       </c>
-    </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH27">
+        <v>25</v>
+      </c>
+      <c r="AI27">
+        <f t="shared" si="1"/>
+        <v>-6.6</v>
+      </c>
+      <c r="AJ27">
+        <f t="shared" si="2"/>
+        <v>-11.9</v>
+      </c>
+      <c r="AK27">
+        <f t="shared" si="3"/>
+        <v>-14.399999999999999</v>
+      </c>
+      <c r="AL27">
+        <f t="shared" si="4"/>
+        <v>3.85</v>
+      </c>
+      <c r="AM27">
+        <f t="shared" si="5"/>
+        <v>12.95</v>
+      </c>
+      <c r="AN27">
+        <f t="shared" si="6"/>
+        <v>14.3</v>
+      </c>
+      <c r="AO27">
+        <f t="shared" si="7"/>
+        <v>22.2</v>
+      </c>
+      <c r="AP27">
+        <f t="shared" si="8"/>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="AQ27">
+        <f t="shared" si="9"/>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="AR27">
+        <f t="shared" si="10"/>
+        <v>-4.25</v>
+      </c>
+      <c r="AS27">
+        <f t="shared" si="11"/>
+        <v>-4.7</v>
+      </c>
+      <c r="AT27">
+        <f t="shared" si="12"/>
+        <v>-8.25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>26</v>
       </c>
@@ -12738,8 +14089,59 @@
       <c r="AG28">
         <v>-15.7</v>
       </c>
-    </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH28">
+        <v>26</v>
+      </c>
+      <c r="AI28">
+        <f t="shared" si="1"/>
+        <v>-8.25</v>
+      </c>
+      <c r="AJ28">
+        <f t="shared" si="2"/>
+        <v>-6.8</v>
+      </c>
+      <c r="AK28">
+        <f t="shared" si="3"/>
+        <v>-13.15</v>
+      </c>
+      <c r="AL28">
+        <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+      <c r="AM28">
+        <f t="shared" si="5"/>
+        <v>12.9</v>
+      </c>
+      <c r="AN28">
+        <f t="shared" si="6"/>
+        <v>14.8</v>
+      </c>
+      <c r="AO28">
+        <f t="shared" si="7"/>
+        <v>20.45</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="8"/>
+        <v>13.35</v>
+      </c>
+      <c r="AQ28">
+        <f t="shared" si="9"/>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="AR28">
+        <f t="shared" si="10"/>
+        <v>-2.9</v>
+      </c>
+      <c r="AS28">
+        <f t="shared" si="11"/>
+        <v>-7.65</v>
+      </c>
+      <c r="AT28">
+        <f t="shared" si="12"/>
+        <v>-8.15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>27</v>
       </c>
@@ -12830,8 +14232,59 @@
       <c r="AG29">
         <v>-13.2</v>
       </c>
-    </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH29">
+        <v>27</v>
+      </c>
+      <c r="AI29">
+        <f t="shared" si="1"/>
+        <v>-17.649999999999999</v>
+      </c>
+      <c r="AJ29">
+        <f t="shared" si="2"/>
+        <v>-13.9</v>
+      </c>
+      <c r="AK29">
+        <f t="shared" si="3"/>
+        <v>-10.5</v>
+      </c>
+      <c r="AL29">
+        <f t="shared" si="4"/>
+        <v>3.9</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" si="5"/>
+        <v>8.5</v>
+      </c>
+      <c r="AN29">
+        <f t="shared" si="6"/>
+        <v>14.55</v>
+      </c>
+      <c r="AO29">
+        <f t="shared" si="7"/>
+        <v>15.1</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="8"/>
+        <v>11.2</v>
+      </c>
+      <c r="AQ29">
+        <f t="shared" si="9"/>
+        <v>3.5</v>
+      </c>
+      <c r="AR29">
+        <f t="shared" si="10"/>
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="AS29">
+        <f t="shared" si="11"/>
+        <v>-11.35</v>
+      </c>
+      <c r="AT29">
+        <f t="shared" si="12"/>
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>28</v>
       </c>
@@ -12922,8 +14375,59 @@
       <c r="AG30">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH30">
+        <v>28</v>
+      </c>
+      <c r="AI30">
+        <f t="shared" si="1"/>
+        <v>-13.45</v>
+      </c>
+      <c r="AJ30">
+        <f t="shared" si="2"/>
+        <v>-17.7</v>
+      </c>
+      <c r="AK30">
+        <f t="shared" si="3"/>
+        <v>-9.75</v>
+      </c>
+      <c r="AL30">
+        <f t="shared" si="4"/>
+        <v>4.6499999999999995</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="5"/>
+        <v>13.55</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="6"/>
+        <v>11.5</v>
+      </c>
+      <c r="AO30">
+        <f t="shared" si="7"/>
+        <v>15.9</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="8"/>
+        <v>9.65</v>
+      </c>
+      <c r="AQ30">
+        <f t="shared" si="9"/>
+        <v>1.4</v>
+      </c>
+      <c r="AR30">
+        <f t="shared" si="10"/>
+        <v>-8.4499999999999993</v>
+      </c>
+      <c r="AS30">
+        <f t="shared" si="11"/>
+        <v>-9.5</v>
+      </c>
+      <c r="AT30">
+        <f t="shared" si="12"/>
+        <v>-10.6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>29</v>
       </c>
@@ -13008,8 +14512,55 @@
       <c r="AG31">
         <v>-7.1</v>
       </c>
-    </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH31">
+        <v>29</v>
+      </c>
+      <c r="AI31">
+        <f t="shared" si="1"/>
+        <v>-9.35</v>
+      </c>
+      <c r="AK31">
+        <f t="shared" si="3"/>
+        <v>-2.6</v>
+      </c>
+      <c r="AL31">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="5"/>
+        <v>15.25</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="6"/>
+        <v>11.5</v>
+      </c>
+      <c r="AO31">
+        <f t="shared" si="7"/>
+        <v>18.149999999999999</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="8"/>
+        <v>10.9</v>
+      </c>
+      <c r="AQ31">
+        <f t="shared" si="9"/>
+        <v>-1.3000000000000003</v>
+      </c>
+      <c r="AR31">
+        <f t="shared" si="10"/>
+        <v>-10.85</v>
+      </c>
+      <c r="AS31">
+        <f t="shared" si="11"/>
+        <v>-2.9000000000000004</v>
+      </c>
+      <c r="AT31">
+        <f t="shared" si="12"/>
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>30</v>
       </c>
@@ -13094,8 +14645,55 @@
       <c r="AG32">
         <v>-14.3</v>
       </c>
-    </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH32">
+        <v>30</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="1"/>
+        <v>-6.75</v>
+      </c>
+      <c r="AK32">
+        <f t="shared" si="3"/>
+        <v>-5.9</v>
+      </c>
+      <c r="AL32">
+        <f t="shared" si="4"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="5"/>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="6"/>
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="7"/>
+        <v>21.35</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="8"/>
+        <v>12.55</v>
+      </c>
+      <c r="AQ32">
+        <f t="shared" si="9"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="AR32">
+        <f t="shared" si="10"/>
+        <v>-11.05</v>
+      </c>
+      <c r="AS32">
+        <f t="shared" si="11"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AT32">
+        <f t="shared" si="12"/>
+        <v>-12.35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>31</v>
       </c>
@@ -13150,8 +14748,35 @@
       <c r="AG33">
         <v>-28</v>
       </c>
-    </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AH33">
+        <v>31</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="1"/>
+        <v>-14.700000000000001</v>
+      </c>
+      <c r="AK33">
+        <f t="shared" si="3"/>
+        <v>-4.1500000000000004</v>
+      </c>
+      <c r="AO33">
+        <f t="shared" si="7"/>
+        <v>23.25</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="8"/>
+        <v>13.35</v>
+      </c>
+      <c r="AR33">
+        <f t="shared" si="10"/>
+        <v>-3.9000000000000004</v>
+      </c>
+      <c r="AT33">
+        <f t="shared" si="12"/>
+        <v>-14.8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD34">
         <v>33</v>
       </c>
@@ -13165,7 +14790,7 @@
         <v>-21.4</v>
       </c>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD35">
         <v>34</v>
       </c>
@@ -13179,7 +14804,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD36">
         <v>35</v>
       </c>
@@ -13193,7 +14818,7 @@
         <v>-23.3</v>
       </c>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD37">
         <v>36</v>
       </c>
@@ -13207,7 +14832,7 @@
         <v>-27.1</v>
       </c>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD38">
         <v>37</v>
       </c>
@@ -13221,7 +14846,7 @@
         <v>-21.5</v>
       </c>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD39">
         <v>38</v>
       </c>
@@ -13235,7 +14860,7 @@
         <v>-15.7</v>
       </c>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD40">
         <v>39</v>
       </c>
@@ -13249,7 +14874,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD41">
         <v>40</v>
       </c>
@@ -13263,7 +14888,7 @@
         <v>-6.3</v>
       </c>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD42">
         <v>41</v>
       </c>
@@ -13277,7 +14902,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD43">
         <v>42</v>
       </c>
@@ -13291,7 +14916,7 @@
         <v>-8.3000000000000007</v>
       </c>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD44">
         <v>43</v>
       </c>
@@ -13305,7 +14930,7 @@
         <v>-12.9</v>
       </c>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD45">
         <v>44</v>
       </c>
@@ -13319,7 +14944,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="46" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD46">
         <v>45</v>
       </c>
@@ -13333,7 +14958,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="47" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD47">
         <v>46</v>
       </c>
@@ -13347,7 +14972,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="48" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:46" x14ac:dyDescent="0.3">
       <c r="AD48">
         <v>47</v>
       </c>
@@ -17783,43 +19408,15 @@
     </row>
     <row r="366" spans="30:33" x14ac:dyDescent="0.3">
       <c r="AD366">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AE366">
-        <v>-23.8</v>
+        <v>-24.7</v>
       </c>
       <c r="AF366">
-        <v>-0.9</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="AG366">
-        <v>-15.4</v>
-      </c>
-    </row>
-    <row r="367" spans="30:33" x14ac:dyDescent="0.3">
-      <c r="AD367">
-        <v>365</v>
-      </c>
-      <c r="AE367">
-        <v>-24.7</v>
-      </c>
-      <c r="AF367">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="AG367">
-        <v>-12.8</v>
-      </c>
-    </row>
-    <row r="368" spans="30:33" x14ac:dyDescent="0.3">
-      <c r="AD368">
-        <v>365</v>
-      </c>
-      <c r="AE368">
-        <v>-24.7</v>
-      </c>
-      <c r="AF368">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="AG368">
         <v>-12.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correction bug pendant la présentation
</commit_message>
<xml_diff>
--- a/Savukoski_kirkonkyla.xlsx
+++ b/Savukoski_kirkonkyla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TP_QualiteDesDonnees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B752B-B82B-4BFC-835B-ABA24BAFD073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145CC423-DDA9-4344-AFAB-3588B5F34846}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="76">
   <si>
     <t>Observation station</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>décembre_median</t>
+  </si>
+  <si>
+    <t>ere</t>
+  </si>
+  <si>
+    <t>erer</t>
   </si>
 </sst>
 </file>
@@ -761,8 +767,8 @@
   <sheetPr codeName="Observation data"/>
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F366"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10283,8 +10289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655AA9EA-45A1-4433-AD1D-A9EF4F799619}">
   <dimension ref="B1:AT366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AO21" sqref="AO21"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AP24" sqref="AP24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13129,6 +13135,9 @@
         <f t="shared" si="6"/>
         <v>15.5</v>
       </c>
+      <c r="AO21" t="s">
+        <v>74</v>
+      </c>
       <c r="AP21">
         <f t="shared" si="8"/>
         <v>14.700000000000001</v>
@@ -13261,6 +13270,9 @@
       <c r="AN22">
         <f t="shared" si="6"/>
         <v>12.85</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>75</v>
       </c>
       <c r="AP22">
         <f t="shared" si="8"/>

</xml_diff>